<commit_message>
Inventory API tests commit along with updated readMe.
</commit_message>
<xml_diff>
--- a/TakeHomeTest_InventoryAPI.xlsx
+++ b/TakeHomeTest_InventoryAPI.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himanshu-g-lnu\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
@@ -17,9 +12,9 @@
     <sheet name="TestEnvironment" sheetId="3" r:id="rId3"/>
     <sheet name="RunTestSuite" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -265,11 +260,6 @@
   </si>
   <si>
     <t>Incorrect method error</t>
-  </si>
-  <si>
-    <t>Update Inventory(UE):-  Method:POST , EndPoint:/update/inventory
-Pre-Requisite: 1.) Connection b/w host and server is established
-2.) DB Access is granted</t>
   </si>
   <si>
     <t>UE_TC-P-01</t>
@@ -1055,12 +1045,17 @@
   <si>
     <t>E2E</t>
   </si>
+  <si>
+    <t>Update Inventory(UE):-  Method:POST , EndPoint:/update/inventory 
+Pre-Requisite: 1.) Connection b/w host and server is established
+2.) DB Access is granted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1145,12 +1140,6 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1169,21 +1158,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1245,7 +1240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1280,7 +1275,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1457,492 +1452,492 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:7" s="7" customFormat="1">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F4">
         <v>200</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="120">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5">
         <v>200</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="75">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F6">
         <v>200</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F7">
         <v>200</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="75">
       <c r="A8" t="s">
         <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F8">
         <v>200</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75">
       <c r="A9" t="s">
         <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F9">
         <v>200</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G9" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60">
       <c r="A10" t="s">
         <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F10">
         <v>401</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60">
       <c r="A11" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F11">
         <v>400</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G11" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="75">
       <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F12">
         <v>400</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60">
       <c r="A13" t="s">
         <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F13">
         <v>400</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" t="s">
         <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F14">
         <v>400</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75">
       <c r="A15" t="s">
         <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="F15">
         <v>400</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G15" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60">
       <c r="A16" t="s">
         <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F16">
         <v>403</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60">
       <c r="A17" t="s">
         <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F17">
         <v>404</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="75">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F18">
         <v>405</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="9" customFormat="1" ht="15.75">
+      <c r="A20" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" ht="105">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F21">
         <v>200</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E22" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F22">
         <v>200</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G22" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
-      </c>
-      <c r="C23" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F23">
         <v>200</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>206</v>
+      <c r="G23" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1956,14 +1951,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
@@ -1974,577 +1969,577 @@
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A1" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="11" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>100</v>
+      <c r="E3" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="165">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>101</v>
+      <c r="C4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="F4">
         <v>201</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="150">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="F5">
         <v>201</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="150">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="F6">
         <v>201</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="135">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>126</v>
+      <c r="E7" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="F7">
         <v>201</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="225">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>127</v>
+      <c r="E8" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F8">
         <v>201</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="165">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>137</v>
+      <c r="D9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="F9">
         <v>401</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="165">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>138</v>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="F10">
         <v>400</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="165">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>139</v>
+      <c r="D11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="F11">
         <v>400</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="165">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>140</v>
+      <c r="E12" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="F12">
         <v>400</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="165">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>141</v>
+      <c r="E13" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="F13">
         <v>400</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="135">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>142</v>
+      <c r="E14" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="F14">
         <v>400</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="165">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>143</v>
+      <c r="D15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="F15">
         <v>400</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="165">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="F16">
         <v>400</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="165">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="F17">
         <v>400</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="165">
+      <c r="A18" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>152</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>153</v>
+      <c r="D18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="F18">
         <v>403</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="180">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>155</v>
+      <c r="D19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="F19">
         <v>404</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="180">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="F20">
         <v>405</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="9" customFormat="1" ht="15.75">
+      <c r="A23" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="180">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
-      </c>
-      <c r="C24" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>211</v>
+      <c r="E24" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="F24">
         <v>200</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="G24" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="180">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>212</v>
+        <v>196</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="F25">
         <v>200</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="G25" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="180">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>212</v>
+        <v>196</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="F26">
         <v>200</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="G26" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A28" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" ht="255">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="D29" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="E29" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G29" s="5" t="s">
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A31" s="17" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="270">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
-      </c>
-      <c r="C32" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="E32" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2560,168 +2555,168 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.28515625" customWidth="1"/>
     <col min="2" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="4" customFormat="1">
+      <c r="A11" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
         <v>189</v>
       </c>
-      <c r="B14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>179</v>
-      </c>
-      <c r="C17" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C19" t="s">
         <v>182</v>
       </c>
-      <c r="C18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:3">
+      <c r="C20" t="s">
         <v>190</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="45">
+      <c r="A22" s="6" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2731,34 +2726,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="50.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:1" ht="30">
+      <c r="A1" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30">
+      <c r="A2" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:1" ht="30">
+      <c r="A3" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:1" ht="30">
+      <c r="A4" s="3" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>